<commit_message>
additions to plots and libs
</commit_message>
<xml_diff>
--- a/booktab style table latex code creator (2).xlsx
+++ b/booktab style table latex code creator (2).xlsx
@@ -2,27 +2,28 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\MOHSIN work\reports n ppts\tidbit-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11835" firstSheet="3" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="paste_and_adjust" sheetId="4" r:id="rId1"/>
     <sheet name="paste_from_adjusted" sheetId="1" r:id="rId2"/>
     <sheet name="copy_from_here" sheetId="2" r:id="rId3"/>
     <sheet name="copy_from_here_(2)" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="46">
   <si>
     <t>Robot</t>
   </si>
@@ -320,6 +321,33 @@
   <si>
     <t>Heading</t>
   </si>
+  <si>
+    <t>achromatopsia</t>
+  </si>
+  <si>
+    <t>tritaponia</t>
+  </si>
+  <si>
+    <t>deuteranopia</t>
+  </si>
+  <si>
+    <t>protanopia</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>srgb</t>
+  </si>
+  <si>
+    <t>lin-rgb</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
 </sst>
 </file>
 
@@ -384,7 +412,7 @@
       <name val="Liberation Sans"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -433,6 +461,30 @@
         <bgColor rgb="FFD9D9D9"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF1A340"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF998EC3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -471,7 +523,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="164" fontId="3" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -490,6 +542,24 @@
     <xf numFmtId="0" fontId="7" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="cf1" xfId="1"/>
@@ -519,6 +589,12 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF998EC3"/>
+      <color rgb="FFF1A340"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -793,6 +869,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet1"/>
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -807,6 +884,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -920,6 +998,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:T67"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -5048,9 +5127,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:U72"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
@@ -9926,4 +10006,456 @@
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr codeName="Sheet5"/>
+  <dimension ref="B1:R25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13:E15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="16384" width="9" style="18"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:18">
+      <c r="C1" s="23"/>
+    </row>
+    <row r="2" spans="2:18">
+      <c r="B2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" s="19"/>
+      <c r="F2" s="19"/>
+      <c r="H2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="I2" s="19"/>
+      <c r="J2" s="19"/>
+      <c r="L2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="M2" s="19"/>
+      <c r="N2" s="19"/>
+      <c r="P2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q2" s="19"/>
+      <c r="R2" s="19"/>
+    </row>
+    <row r="3" spans="2:18">
+      <c r="B3" s="18">
+        <v>84</v>
+      </c>
+      <c r="D3" s="18">
+        <v>0.17055999999999999</v>
+      </c>
+      <c r="E3" s="18">
+        <v>0.82943999999999996</v>
+      </c>
+      <c r="F3" s="18">
+        <v>0</v>
+      </c>
+      <c r="H3" s="18">
+        <v>0.33066000000000001</v>
+      </c>
+      <c r="I3" s="18">
+        <v>0.66934000000000005</v>
+      </c>
+      <c r="J3" s="18">
+        <v>0</v>
+      </c>
+      <c r="L3" s="18">
+        <v>1</v>
+      </c>
+      <c r="M3" s="18">
+        <v>0.12740000000000001</v>
+      </c>
+      <c r="N3" s="18">
+        <v>-0.12740000000000001</v>
+      </c>
+      <c r="P3" s="18">
+        <v>0.21229999999999999</v>
+      </c>
+      <c r="Q3" s="18">
+        <v>0.71519999999999995</v>
+      </c>
+      <c r="R3" s="18">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:18">
+      <c r="B4" s="18">
+        <v>39</v>
+      </c>
+      <c r="D4" s="18">
+        <v>0.17055999999999999</v>
+      </c>
+      <c r="E4" s="18">
+        <v>0.82943999999999996</v>
+      </c>
+      <c r="F4" s="18">
+        <v>0</v>
+      </c>
+      <c r="H4" s="18">
+        <v>0.33066000000000001</v>
+      </c>
+      <c r="I4" s="18">
+        <v>0.66934000000000005</v>
+      </c>
+      <c r="J4" s="18">
+        <v>0</v>
+      </c>
+      <c r="L4" s="18">
+        <v>0</v>
+      </c>
+      <c r="M4" s="18">
+        <v>0.87390000000000001</v>
+      </c>
+      <c r="N4" s="18">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="P4" s="18">
+        <v>0.21229999999999999</v>
+      </c>
+      <c r="Q4" s="18">
+        <v>0.71519999999999995</v>
+      </c>
+      <c r="R4" s="18">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:18">
+      <c r="B5" s="18">
+        <v>136</v>
+      </c>
+      <c r="D5" s="18">
+        <v>-4.5199999999999997E-3</v>
+      </c>
+      <c r="E5" s="18">
+        <v>4.5199999999999997E-3</v>
+      </c>
+      <c r="F5" s="18">
+        <v>1</v>
+      </c>
+      <c r="H5" s="18">
+        <v>-2.7859999999999999E-2</v>
+      </c>
+      <c r="I5" s="18">
+        <v>2.7859999999999999E-2</v>
+      </c>
+      <c r="J5" s="18">
+        <v>1</v>
+      </c>
+      <c r="L5" s="18">
+        <v>0</v>
+      </c>
+      <c r="M5" s="18">
+        <v>0.87390000000000001</v>
+      </c>
+      <c r="N5" s="18">
+        <v>0.12609999999999999</v>
+      </c>
+      <c r="P5" s="18">
+        <v>0.21229999999999999</v>
+      </c>
+      <c r="Q5" s="18">
+        <v>0.71519999999999995</v>
+      </c>
+      <c r="R5" s="18">
+        <v>7.22E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:18">
+      <c r="B7" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="8" spans="2:18">
+      <c r="B8" s="18">
+        <f>IF( B3/255&lt;=0.04045, B3/255/12.92, POWER((B3/255+0.055)/1.055,2.4) )</f>
+        <v>8.8655586285772928E-2</v>
+      </c>
+      <c r="D8" s="18">
+        <f t="array" ref="D8:D10">MMULT(D3:F5,$B$8:$B$10)</f>
+        <v>3.1949242538611193E-2</v>
+      </c>
+      <c r="E8" s="18">
+        <f>MAX(D8,0)</f>
+        <v>3.1949242538611193E-2</v>
+      </c>
+      <c r="H8" s="18">
+        <f t="array" ref="H8:H10">MMULT(H3:J5,$B$8:$B$10)</f>
+        <v>4.2894802957593396E-2</v>
+      </c>
+      <c r="I8" s="18">
+        <f>MAX(H8,0)</f>
+        <v>4.2894802957593396E-2</v>
+      </c>
+      <c r="L8" s="18">
+        <f t="array" ref="L8:L10">MMULT(L3:N5,$B$8:$B$10)</f>
+        <v>5.9874300196612204E-2</v>
+      </c>
+      <c r="M8" s="18">
+        <f>MAX(L8,0)</f>
+        <v>5.9874300196612204E-2</v>
+      </c>
+      <c r="P8" s="18">
+        <f t="array" ref="P8:P10">MMULT(P3:R5,$B$8:$B$10)</f>
+        <v>5.1107697054893098E-2</v>
+      </c>
+      <c r="Q8" s="18">
+        <f>MAX(P8,0)</f>
+        <v>5.1107697054893098E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="2:18">
+      <c r="B9" s="18">
+        <f t="shared" ref="B9:B10" si="0">IF( B4/255&lt;=0.04045, B4/255/12.92, POWER((B4/255+0.055)/1.055,2.4) )</f>
+        <v>2.0288563056652397E-2</v>
+      </c>
+      <c r="D9" s="18">
+        <v>3.1949242538611193E-2</v>
+      </c>
+      <c r="E9" s="18">
+        <f t="shared" ref="E9:E10" si="1">MAX(D9,0)</f>
+        <v>3.1949242538611193E-2</v>
+      </c>
+      <c r="H9" s="18">
+        <v>4.2894802957593396E-2</v>
+      </c>
+      <c r="I9" s="18">
+        <f t="shared" ref="I9:I10" si="2">MAX(H9,0)</f>
+        <v>4.2894802957593396E-2</v>
+      </c>
+      <c r="L9" s="18">
+        <v>4.8776162553066577E-2</v>
+      </c>
+      <c r="M9" s="18">
+        <f t="shared" ref="M9:M10" si="3">MAX(L9,0)</f>
+        <v>4.8776162553066577E-2</v>
+      </c>
+      <c r="P9" s="18">
+        <v>5.1107697054893098E-2</v>
+      </c>
+      <c r="Q9" s="18">
+        <f t="shared" ref="Q9:Q10" si="4">MAX(P9,0)</f>
+        <v>5.1107697054893098E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:18">
+      <c r="B10" s="18">
+        <f t="shared" si="0"/>
+        <v>0.24620132670783543</v>
+      </c>
+      <c r="D10" s="18">
+        <v>0.2458923077628398</v>
+      </c>
+      <c r="E10" s="18">
+        <f t="shared" si="1"/>
+        <v>0.2458923077628398</v>
+      </c>
+      <c r="H10" s="18">
+        <v>0.24429662144067213</v>
+      </c>
+      <c r="I10" s="18">
+        <f t="shared" si="2"/>
+        <v>0.24429662144067213</v>
+      </c>
+      <c r="L10" s="18">
+        <v>4.8776162553066577E-2</v>
+      </c>
+      <c r="M10" s="18">
+        <f t="shared" si="3"/>
+        <v>4.8776162553066577E-2</v>
+      </c>
+      <c r="P10" s="18">
+        <v>5.1107697054893098E-2</v>
+      </c>
+      <c r="Q10" s="18">
+        <f t="shared" si="4"/>
+        <v>5.1107697054893098E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18">
+      <c r="B13" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="D13" s="18">
+        <f>IF( E8&lt;=0.0031308, 255*12.92*E8, 255*( 1.055*POWER(E8,1/2.4)-0.055 ) )</f>
+        <v>50.044481496774118</v>
+      </c>
+      <c r="E13" s="18">
+        <f>ROUND(D13,)</f>
+        <v>50</v>
+      </c>
+      <c r="H13" s="18">
+        <f>IF( I8&lt;=0.0031308, 255*12.92*I8, 255*( 1.055*POWER(I8,1/2.4)-0.055 ) )</f>
+        <v>58.412133430998907</v>
+      </c>
+      <c r="L13" s="18">
+        <f>IF( M8&lt;=0.0031308, 255*12.92*M8, 255*( 1.055*POWER(M8,1/2.4)-0.055 ) )</f>
+        <v>69.210672821693279</v>
+      </c>
+      <c r="P13" s="18">
+        <f>IF( Q8&lt;=0.0031308, 255*12.92*Q8, 255*( 1.055*POWER(Q8,1/2.4)-0.055 ) )</f>
+        <v>63.897331167085703</v>
+      </c>
+    </row>
+    <row r="14" spans="2:18">
+      <c r="D14" s="18">
+        <f t="shared" ref="D14:D15" si="5">IF( E9&lt;=0.0031308, 255*12.92*E9, 255*( 1.055*POWER(E9,1/2.4)-0.055 ) )</f>
+        <v>50.044481496774118</v>
+      </c>
+      <c r="E14" s="18">
+        <f t="shared" ref="E14:E15" si="6">ROUND(D14,)</f>
+        <v>50</v>
+      </c>
+      <c r="F14" s="18" t="e">
+        <f ca="1">GetFillColor(E13,E14,E15)</f>
+        <v>#NAME?</v>
+      </c>
+      <c r="H14" s="18">
+        <f t="shared" ref="H14:H15" si="7">IF( I9&lt;=0.0031308, 255*12.92*I9, 255*( 1.055*POWER(I9,1/2.4)-0.055 ) )</f>
+        <v>58.412133430998907</v>
+      </c>
+      <c r="L14" s="18">
+        <f t="shared" ref="L14:L15" si="8">IF( M9&lt;=0.0031308, 255*12.92*M9, 255*( 1.055*POWER(M9,1/2.4)-0.055 ) )</f>
+        <v>62.39595940896465</v>
+      </c>
+      <c r="P14" s="18">
+        <f t="shared" ref="P14:P15" si="9">IF( Q9&lt;=0.0031308, 255*12.92*Q9, 255*( 1.055*POWER(Q9,1/2.4)-0.055 ) )</f>
+        <v>63.897331167085703</v>
+      </c>
+    </row>
+    <row r="15" spans="2:18">
+      <c r="D15" s="18">
+        <f t="shared" si="5"/>
+        <v>135.9215114736468</v>
+      </c>
+      <c r="E15" s="18">
+        <f t="shared" si="6"/>
+        <v>136</v>
+      </c>
+      <c r="H15" s="18">
+        <f t="shared" si="7"/>
+        <v>135.51530040560621</v>
+      </c>
+      <c r="L15" s="18">
+        <f t="shared" si="8"/>
+        <v>62.39595940896465</v>
+      </c>
+      <c r="P15" s="18">
+        <f t="shared" si="9"/>
+        <v>63.897331167085703</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5">
+      <c r="C18" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="E18" s="18" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5">
+      <c r="C19" s="18">
+        <v>179</v>
+      </c>
+      <c r="D19" s="18">
+        <v>88</v>
+      </c>
+      <c r="E19" s="18">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="20" spans="2:5">
+      <c r="B20" s="20"/>
+      <c r="C20" s="18">
+        <v>241</v>
+      </c>
+      <c r="D20" s="18">
+        <v>163</v>
+      </c>
+      <c r="E20" s="18">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="21" spans="2:5">
+      <c r="C21" s="18">
+        <v>253</v>
+      </c>
+      <c r="D21" s="18">
+        <v>184</v>
+      </c>
+      <c r="E21" s="18">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="22" spans="2:5">
+      <c r="B22" s="21"/>
+      <c r="C22" s="18">
+        <v>247</v>
+      </c>
+      <c r="D22" s="18">
+        <v>247</v>
+      </c>
+      <c r="E22" s="18">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="23" spans="2:5">
+      <c r="C23" s="18">
+        <v>178</v>
+      </c>
+      <c r="D23" s="18">
+        <v>171</v>
+      </c>
+      <c r="E23" s="18">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="24" spans="2:5">
+      <c r="B24" s="22"/>
+      <c r="C24" s="18">
+        <v>153</v>
+      </c>
+      <c r="D24" s="18">
+        <v>142</v>
+      </c>
+      <c r="E24" s="18">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="25" spans="2:5">
+      <c r="C25" s="18">
+        <v>84</v>
+      </c>
+      <c r="D25" s="18">
+        <v>39</v>
+      </c>
+      <c r="E25" s="18">
+        <v>136</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="D2:F2"/>
+    <mergeCell ref="H2:J2"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="P2:R2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="landscape" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>